<commit_message>
FIX not reading data as str
It breaks the output data type which is not good.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -476,10 +476,8 @@
           <t>Female</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
+      <c r="D2" t="n">
+        <v>21</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -503,10 +501,8 @@
           <t>Male</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
+      <c r="D3" t="n">
+        <v>19</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -530,10 +526,8 @@
           <t>Female</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
+      <c r="D4" t="n">
+        <v>28</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -557,10 +551,8 @@
           <t>Male</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+      <c r="D5" t="n">
+        <v>29</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -584,10 +576,8 @@
           <t>Female</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
+      <c r="D6" t="n">
+        <v>26</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -611,10 +601,8 @@
           <t>Female</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
+      <c r="D7" t="n">
+        <v>22</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -638,10 +626,8 @@
           <t>Female</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+      <c r="D8" t="n">
+        <v>30</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -665,10 +651,8 @@
           <t>Male</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="D9" t="n">
+        <v>25</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -692,10 +676,8 @@
           <t>Female</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
+      <c r="D10" t="n">
+        <v>19</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -719,10 +701,8 @@
           <t>Female</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="D11" t="n">
+        <v>20</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>

</xml_diff>